<commit_message>
Added default wargear data to xlsx files and modified unit data class to use it
</commit_message>
<xml_diff>
--- a/Necron_units.xlsx
+++ b/Necron_units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Warhammer\Army Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A8849FB-9956-48AF-A1C7-D0B40DDA891D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A33EC02-AEF9-4C6B-9D71-4503B33FFD77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="7" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="6" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Named Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>Anrakyr the Traveller</t>
   </si>
@@ -167,6 +167,75 @@
   </si>
   <si>
     <t>Night Scythe</t>
+  </si>
+  <si>
+    <t>Wargear</t>
+  </si>
+  <si>
+    <t>Gauss cannon, Staff of light</t>
+  </si>
+  <si>
+    <t>Staff of light</t>
+  </si>
+  <si>
+    <t>Gauss blaster</t>
+  </si>
+  <si>
+    <t>Gauss flayer</t>
+  </si>
+  <si>
+    <t>Synaptic disintergrator</t>
+  </si>
+  <si>
+    <t>Flayer claws</t>
+  </si>
+  <si>
+    <t>Rod of covenant</t>
+  </si>
+  <si>
+    <t>Warscythe</t>
+  </si>
+  <si>
+    <t>Heat ray, Massive forelimbs</t>
+  </si>
+  <si>
+    <t>Feeder mandibles</t>
+  </si>
+  <si>
+    <t>Viscious claws</t>
+  </si>
+  <si>
+    <t>Gauss cannon</t>
+  </si>
+  <si>
+    <t>2 Gauss blasters</t>
+  </si>
+  <si>
+    <t>Automaton claws</t>
+  </si>
+  <si>
+    <t>Gauss cannon, Twin tesla destructor</t>
+  </si>
+  <si>
+    <t>Heavy gauss cannon</t>
+  </si>
+  <si>
+    <t>Crackling tendrils</t>
+  </si>
+  <si>
+    <t>2*Gauss flayer arrays</t>
+  </si>
+  <si>
+    <t>4*Gauss flux arcs, Particle whip</t>
+  </si>
+  <si>
+    <t>2*Gauss flayer arrays, Doomsday cannon</t>
+  </si>
+  <si>
+    <t>2*Tesla destructors, Death ray</t>
+  </si>
+  <si>
+    <t>2*Tesla destructors</t>
   </si>
 </sst>
 </file>
@@ -519,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7F590D-8B75-4D8D-9044-3256E0122977}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +601,7 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -542,8 +611,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -554,7 +626,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -565,7 +637,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -576,7 +648,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -587,7 +659,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -598,7 +670,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -609,7 +681,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -620,7 +692,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -631,7 +703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -649,18 +721,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE43A1E-BCF6-491A-9639-47067C57DF8D}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -670,8 +744,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -681,8 +758,11 @@
       <c r="C2">
         <v>138</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -692,8 +772,11 @@
       <c r="C3">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -703,8 +786,11 @@
       <c r="C4">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -714,8 +800,11 @@
       <c r="C5">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -724,6 +813,9 @@
       </c>
       <c r="C6">
         <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -733,10 +825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F0D7BD-74BE-4ECF-BAFB-BB62C0A6B8FC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +838,7 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -756,8 +848,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -767,8 +862,11 @@
       <c r="C2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -777,6 +875,9 @@
       </c>
       <c r="C3">
         <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -787,10 +888,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC447E6-11FB-459C-9327-A7E9F0B0862D}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +901,7 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -810,8 +911,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -821,8 +925,11 @@
       <c r="C2">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -832,8 +939,11 @@
       <c r="C3">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -843,8 +953,11 @@
       <c r="C4">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -854,8 +967,11 @@
       <c r="C5">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -864,6 +980,9 @@
       </c>
       <c r="C6">
         <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -876,19 +995,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4BF480-01AD-407E-A47E-AFEB6F430058}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -898,8 +1018,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -909,8 +1032,11 @@
       <c r="C2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -920,8 +1046,11 @@
       <c r="C3">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -931,8 +1060,11 @@
       <c r="C4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -941,6 +1073,9 @@
       </c>
       <c r="C5">
         <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -950,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2FD502-0F4A-4383-8D36-7E1605FC681F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +1097,7 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -973,7 +1108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -983,8 +1118,11 @@
       <c r="C2">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -994,8 +1132,11 @@
       <c r="C3">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1005,8 +1146,11 @@
       <c r="C4">
         <v>193</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1016,8 +1160,11 @@
       <c r="C5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1027,8 +1174,11 @@
       <c r="C6">
         <v>381</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1037,6 +1187,9 @@
       </c>
       <c r="C7">
         <v>225</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1046,15 +1199,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3774BF29-A26D-4C9B-BAC4-736D4BBB0B22}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1064,8 +1217,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1074,6 +1230,9 @@
       </c>
       <c r="C2">
         <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1083,15 +1242,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B9CEA0-6C93-4328-A414-30C4B33A5DEC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1101,8 +1260,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1112,8 +1274,11 @@
       <c r="C2">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1122,6 +1287,9 @@
       </c>
       <c r="C3">
         <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified unit listings to calculate the base number of points per model with default wargear and minimum points per unit
</commit_message>
<xml_diff>
--- a/Necron_units.xlsx
+++ b/Necron_units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Warhammer\Army Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A33EC02-AEF9-4C6B-9D71-4503B33FFD77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2B9D11CF-C7DD-4146-B2C9-3FCFD51763D7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="6" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="3" activeTab="6" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Named Characters" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>Gauss flayer</t>
   </si>
   <si>
-    <t>Synaptic disintergrator</t>
-  </si>
-  <si>
     <t>Flayer claws</t>
   </si>
   <si>
@@ -202,15 +199,9 @@
     <t>Feeder mandibles</t>
   </si>
   <si>
-    <t>Viscious claws</t>
-  </si>
-  <si>
     <t>Gauss cannon</t>
   </si>
   <si>
-    <t>2 Gauss blasters</t>
-  </si>
-  <si>
     <t>Automaton claws</t>
   </si>
   <si>
@@ -223,19 +214,28 @@
     <t>Crackling tendrils</t>
   </si>
   <si>
-    <t>2*Gauss flayer arrays</t>
-  </si>
-  <si>
-    <t>4*Gauss flux arcs, Particle whip</t>
-  </si>
-  <si>
-    <t>2*Gauss flayer arrays, Doomsday cannon</t>
-  </si>
-  <si>
-    <t>2*Tesla destructors, Death ray</t>
-  </si>
-  <si>
-    <t>2*Tesla destructors</t>
+    <t>2*Gauss flayer array, Doomsday cannon</t>
+  </si>
+  <si>
+    <t>4*Gauss flux arc, Particle whip</t>
+  </si>
+  <si>
+    <t>2*Tesla destructor, Death ray</t>
+  </si>
+  <si>
+    <t>2*Tesla destructor</t>
+  </si>
+  <si>
+    <t>Vicious claws</t>
+  </si>
+  <si>
+    <t>2*Gauss blaster</t>
+  </si>
+  <si>
+    <t>Synaptic disintegrator</t>
+  </si>
+  <si>
+    <t>2*Gauss flayer array</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +926,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
         <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1061,7 +1061,7 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1119,7 @@
         <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,7 +1133,7 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1175,7 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>225</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1202,7 +1202,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,7 +1232,7 @@
         <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1245,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1275,7 @@
         <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
         <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional tests, and began developing wargear options for units class
</commit_message>
<xml_diff>
--- a/Necron_units.xlsx
+++ b/Necron_units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Warhammer\Army Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2B9D11CF-C7DD-4146-B2C9-3FCFD51763D7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{969E248D-A1A4-4F03-A668-C508C488B819}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="3" activeTab="6" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Named Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
   <si>
     <t>Anrakyr the Traveller</t>
   </si>
@@ -187,55 +187,91 @@
     <t>Flayer claws</t>
   </si>
   <si>
+    <t>Heat ray, Massive forelimbs</t>
+  </si>
+  <si>
+    <t>Feeder mandibles</t>
+  </si>
+  <si>
+    <t>Gauss cannon</t>
+  </si>
+  <si>
+    <t>Automaton claws</t>
+  </si>
+  <si>
+    <t>Gauss cannon, Twin tesla destructor</t>
+  </si>
+  <si>
+    <t>Heavy gauss cannon</t>
+  </si>
+  <si>
+    <t>Crackling tendrils</t>
+  </si>
+  <si>
+    <t>2*Gauss flayer array, Doomsday cannon</t>
+  </si>
+  <si>
+    <t>4*Gauss flux arc, Particle whip</t>
+  </si>
+  <si>
+    <t>2*Tesla destructor, Death ray</t>
+  </si>
+  <si>
+    <t>2*Tesla destructor</t>
+  </si>
+  <si>
+    <t>Vicious claws</t>
+  </si>
+  <si>
+    <t>2*Gauss blaster</t>
+  </si>
+  <si>
+    <t>Synaptic disintegrator</t>
+  </si>
+  <si>
+    <t>2*Gauss flayer array</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Gauss cannon/Tesla cannon</t>
+  </si>
+  <si>
+    <t>Gloom prism, Fabricator claw array</t>
+  </si>
+  <si>
+    <t>Whip coils, Transdimensional beamer/Particle caster</t>
+  </si>
+  <si>
+    <t>Heavy gauss cannon-3</t>
+  </si>
+  <si>
+    <t>Shieldvanes, Nebuloscope/Shadowloom</t>
+  </si>
+  <si>
+    <t>Warscythe/Hyperphase sword+Dispersion shield</t>
+  </si>
+  <si>
+    <t>Rod of the covennant/Particle caster+Voidblade</t>
+  </si>
+  <si>
+    <t>Heat Ray/2*Heavy gauss cannon/Particle Shredder</t>
+  </si>
+  <si>
+    <t>Tesla Cannon, Staff of light/Warscythe/Hyperphase sword/Voidblade/, Phylactery, Resurrection orb</t>
+  </si>
+  <si>
+    <t>Phylactery, Canoptek Cloak/Chronometron</t>
+  </si>
+  <si>
+    <t>Staff of light/Warscythe/Hyperphase sword/Voidblade/, Phylactery, Resurrection orb</t>
+  </si>
+  <si>
+    <t>Warscythe</t>
+  </si>
+  <si>
     <t>Rod of covenant</t>
-  </si>
-  <si>
-    <t>Warscythe</t>
-  </si>
-  <si>
-    <t>Heat ray, Massive forelimbs</t>
-  </si>
-  <si>
-    <t>Feeder mandibles</t>
-  </si>
-  <si>
-    <t>Gauss cannon</t>
-  </si>
-  <si>
-    <t>Automaton claws</t>
-  </si>
-  <si>
-    <t>Gauss cannon, Twin tesla destructor</t>
-  </si>
-  <si>
-    <t>Heavy gauss cannon</t>
-  </si>
-  <si>
-    <t>Crackling tendrils</t>
-  </si>
-  <si>
-    <t>2*Gauss flayer array, Doomsday cannon</t>
-  </si>
-  <si>
-    <t>4*Gauss flux arc, Particle whip</t>
-  </si>
-  <si>
-    <t>2*Tesla destructor, Death ray</t>
-  </si>
-  <si>
-    <t>2*Tesla destructor</t>
-  </si>
-  <si>
-    <t>Vicious claws</t>
-  </si>
-  <si>
-    <t>2*Gauss blaster</t>
-  </si>
-  <si>
-    <t>Synaptic disintegrator</t>
-  </si>
-  <si>
-    <t>2*Gauss flayer array</t>
   </si>
 </sst>
 </file>
@@ -588,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7F590D-8B75-4D8D-9044-3256E0122977}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +637,7 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -614,8 +650,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -626,7 +665,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -637,7 +676,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -648,7 +687,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -659,7 +698,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -670,7 +709,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -681,7 +720,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -692,7 +731,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -703,7 +742,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -721,10 +760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE43A1E-BCF6-491A-9639-47067C57DF8D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,9 +771,10 @@
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -747,8 +787,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -761,8 +804,11 @@
       <c r="D2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -775,8 +821,11 @@
       <c r="D3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -789,8 +838,11 @@
       <c r="D4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -803,8 +855,11 @@
       <c r="D5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -816,6 +871,9 @@
       </c>
       <c r="D6" t="s">
         <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -825,10 +883,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F0D7BD-74BE-4ECF-BAFB-BB62C0A6B8FC}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,9 +894,10 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -851,8 +910,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -866,7 +928,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -888,10 +950,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC447E6-11FB-459C-9327-A7E9F0B0862D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,9 +961,10 @@
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -914,8 +977,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -926,10 +992,10 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -943,7 +1009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -954,10 +1020,13 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -968,10 +1037,13 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -982,7 +1054,10 @@
         <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -995,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4BF480-01AD-407E-A47E-AFEB6F430058}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,9 +1081,10 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1021,8 +1097,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1033,10 +1112,10 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1047,10 +1126,13 @@
         <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1061,10 +1143,13 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1075,7 +1160,10 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1085,19 +1173,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2FD502-0F4A-4383-8D36-7E1605FC681F}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1107,8 +1197,14 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1119,10 +1215,13 @@
         <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1133,10 +1232,13 @@
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1147,10 +1249,10 @@
         <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1161,10 +1263,10 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1175,10 +1277,10 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1189,7 +1291,7 @@
         <v>225</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1199,15 +1301,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3774BF29-A26D-4C9B-BAC4-736D4BBB0B22}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1220,8 +1325,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1232,7 +1340,7 @@
         <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1242,15 +1350,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B9CEA0-6C93-4328-A414-30C4B33A5DEC}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1263,8 +1371,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1275,10 +1386,10 @@
         <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1289,7 +1400,7 @@
         <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created tests to check errors in Necron_units file as well as split up the global variables and classes into an init file
</commit_message>
<xml_diff>
--- a/Necron_units.xlsx
+++ b/Necron_units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Warhammer\Army Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{969E248D-A1A4-4F03-A668-C508C488B819}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD87FE49-FBA9-4FE2-AF8C-78546B0048FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{8DE1005F-ABA0-47E0-93D2-7C531C6189BE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>Anrakyr the Traveller</t>
   </si>
@@ -244,34 +244,37 @@
     <t>Whip coils, Transdimensional beamer/Particle caster</t>
   </si>
   <si>
-    <t>Heavy gauss cannon-3</t>
-  </si>
-  <si>
     <t>Shieldvanes, Nebuloscope/Shadowloom</t>
   </si>
   <si>
     <t>Warscythe/Hyperphase sword+Dispersion shield</t>
   </si>
   <si>
-    <t>Rod of the covennant/Particle caster+Voidblade</t>
-  </si>
-  <si>
-    <t>Heat Ray/2*Heavy gauss cannon/Particle Shredder</t>
-  </si>
-  <si>
-    <t>Tesla Cannon, Staff of light/Warscythe/Hyperphase sword/Voidblade/, Phylactery, Resurrection orb</t>
-  </si>
-  <si>
-    <t>Phylactery, Canoptek Cloak/Chronometron</t>
-  </si>
-  <si>
-    <t>Staff of light/Warscythe/Hyperphase sword/Voidblade/, Phylactery, Resurrection orb</t>
-  </si>
-  <si>
     <t>Warscythe</t>
   </si>
   <si>
     <t>Rod of covenant</t>
+  </si>
+  <si>
+    <t>Gauss blaster/Tesla carbine</t>
+  </si>
+  <si>
+    <t>Gauss cannon/Heavy gauss cannon-3</t>
+  </si>
+  <si>
+    <t>Gauss cannon/Tesla cannon, Staff of light/Warscythe/Hyperphase sword/Voidblade, Phylactery, Resurrection orb</t>
+  </si>
+  <si>
+    <t>Staff of light/Warscythe/Hyperphase sword/Voidblade, Phylactery, Resurrection orb</t>
+  </si>
+  <si>
+    <t>Phylactery, Canoptek cloak/Chronometron</t>
+  </si>
+  <si>
+    <t>Rod of covenant/Particle caster+Voidblade</t>
+  </si>
+  <si>
+    <t>Heat ray/2*Heavy gauss cannon/Particle shredder</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +808,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,7 +825,7 @@
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -886,7 +889,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +930,9 @@
       <c r="D2" t="s">
         <v>48</v>
       </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -953,7 +959,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,10 +1026,10 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,10 +1043,10 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
         <v>79</v>
-      </c>
-      <c r="E5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,7 +1063,7 @@
         <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1079,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1152,7 @@
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,7 +1169,7 @@
         <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>